<commit_message>
Inserção de novas funções e mais funcionalidades de gráficos
</commit_message>
<xml_diff>
--- a/PLANILHA TAF.xlsx
+++ b/PLANILHA TAF.xlsx
@@ -3834,7 +3834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K44" sqref="K44"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14.25"/>
@@ -6802,7 +6802,7 @@
         <v>61</v>
       </c>
       <c r="C52" s="9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>15</v>

</xml_diff>